<commit_message>
Changes Pre Driver Input Changes
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/flyball_governor.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/flyball_governor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C948F7C0-810F-4565-A083-19F02F75C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC0D65F-499B-4DAE-9553-E95652EACA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1301,18 +1301,93 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1331,12 +1406,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1346,74 +1415,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1421,7 +1424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,7 +1433,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1442,15 +1451,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1466,15 +1466,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1494,33 +1521,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1957,7 +1957,7 @@
   <dimension ref="B2:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,44 +1976,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
-      <c r="J2" s="68" t="s">
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
+      <c r="J2" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="71"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="53">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="J3" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="78" t="s">
+      <c r="K3" s="95"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="92"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="77"/>
       <c r="P3" s="47" t="s">
         <v>164</v>
       </c>
@@ -2022,12 +2022,12 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="53">
-        <v>2.9999999999999997E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="E4" s="53" t="s">
         <v>22</v>
@@ -2038,14 +2038,14 @@
       <c r="K4" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="45" t="s">
         <v>134</v>
       </c>
       <c r="N4" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="O4" s="93"/>
+      <c r="O4" s="78"/>
       <c r="P4" s="47" t="s">
         <v>165</v>
       </c>
@@ -2054,10 +2054,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="71"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="53" t="s">
         <v>85</v>
       </c>
@@ -2070,14 +2070,14 @@
       <c r="K5" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="81"/>
+      <c r="L5" s="104"/>
       <c r="M5" s="47" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="93"/>
+      <c r="O5" s="78"/>
       <c r="P5" s="47" t="s">
         <v>166</v>
       </c>
@@ -2086,10 +2086,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="71"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="53" t="s">
         <v>3</v>
       </c>
@@ -2102,14 +2102,14 @@
       <c r="K6" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="81"/>
+      <c r="L6" s="104"/>
       <c r="M6" s="47" t="s">
         <v>136</v>
       </c>
       <c r="N6" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="O6" s="93"/>
+      <c r="O6" s="78"/>
       <c r="P6" s="47" t="s">
         <v>170</v>
       </c>
@@ -2118,10 +2118,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="71"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="53">
         <v>-9806.65</v>
       </c>
@@ -2134,14 +2134,14 @@
       <c r="K7" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="81"/>
+      <c r="L7" s="104"/>
       <c r="M7" s="47" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="93"/>
+      <c r="O7" s="78"/>
       <c r="P7" s="47" t="s">
         <v>169</v>
       </c>
@@ -2150,10 +2150,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="71"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="53" t="s">
         <v>132</v>
       </c>
@@ -2166,14 +2166,14 @@
       <c r="K8" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="81"/>
+      <c r="L8" s="104"/>
       <c r="M8" s="47" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="93"/>
+      <c r="O8" s="78"/>
       <c r="P8" s="47" t="s">
         <v>173</v>
       </c>
@@ -2182,10 +2182,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="71"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="53"/>
       <c r="E9" s="54" t="s">
         <v>126</v>
@@ -2196,14 +2196,14 @@
       <c r="K9" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="L9" s="81"/>
+      <c r="L9" s="104"/>
       <c r="M9" s="47" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="93"/>
+      <c r="O9" s="78"/>
       <c r="P9" s="47" t="s">
         <v>174</v>
       </c>
@@ -2218,14 +2218,14 @@
       <c r="K10" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="L10" s="81"/>
+      <c r="L10" s="104"/>
       <c r="M10" s="47" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="93"/>
+      <c r="O10" s="78"/>
       <c r="P10" s="52" t="s">
         <v>175</v>
       </c>
@@ -2236,14 +2236,14 @@
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J11" s="56"/>
       <c r="K11" s="57"/>
-      <c r="L11" s="81"/>
+      <c r="L11" s="104"/>
       <c r="M11" s="47" t="s">
         <v>138</v>
       </c>
       <c r="N11" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="O11" s="93"/>
+      <c r="O11" s="78"/>
       <c r="P11" s="52" t="s">
         <v>176</v>
       </c>
@@ -2252,25 +2252,25 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="101" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
       <c r="J12" s="58"/>
       <c r="K12" s="59"/>
-      <c r="L12" s="81"/>
+      <c r="L12" s="104"/>
       <c r="M12" s="47" t="s">
         <v>139</v>
       </c>
       <c r="N12" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="O12" s="93"/>
+      <c r="O12" s="78"/>
       <c r="P12" s="47" t="s">
         <v>181</v>
       </c>
@@ -2279,29 +2279,29 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="81"/>
       <c r="D13" s="44" t="s">
         <v>242</v>
       </c>
       <c r="E13" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
       <c r="J13" s="58"/>
       <c r="K13" s="59"/>
-      <c r="L13" s="81"/>
+      <c r="L13" s="104"/>
       <c r="M13" s="47" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="93"/>
+      <c r="O13" s="78"/>
       <c r="P13" s="52" t="s">
         <v>182</v>
       </c>
@@ -2310,27 +2310,27 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="44"/>
       <c r="E14" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="100"/>
       <c r="J14" s="60"/>
       <c r="K14" s="61"/>
-      <c r="L14" s="81"/>
+      <c r="L14" s="104"/>
       <c r="M14" s="47" t="s">
         <v>140</v>
       </c>
       <c r="N14" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="O14" s="93"/>
+      <c r="O14" s="78"/>
       <c r="P14" s="52" t="s">
         <v>183</v>
       </c>
@@ -2339,29 +2339,29 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="44"/>
       <c r="E15" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="J15" s="78" t="s">
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="100"/>
+      <c r="J15" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="79"/>
-      <c r="L15" s="81"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="104"/>
       <c r="M15" s="47" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="93"/>
+      <c r="O15" s="78"/>
       <c r="P15" s="52" t="s">
         <v>184</v>
       </c>
@@ -2370,31 +2370,31 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="69"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="46"/>
       <c r="E16" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
       <c r="J16" s="47" t="s">
         <v>97</v>
       </c>
       <c r="K16" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="L16" s="81"/>
+      <c r="L16" s="104"/>
       <c r="M16" s="47" t="s">
         <v>141</v>
       </c>
       <c r="N16" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="O16" s="93"/>
+      <c r="O16" s="78"/>
       <c r="P16" s="47" t="s">
         <v>189</v>
       </c>
@@ -2403,29 +2403,29 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="69"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="46"/>
       <c r="E17" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
       <c r="J17" s="47" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="L17" s="81"/>
-      <c r="M17" s="78" t="s">
+      <c r="L17" s="104"/>
+      <c r="M17" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="N17" s="79"/>
-      <c r="O17" s="93"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="78"/>
       <c r="P17" s="52" t="s">
         <v>190</v>
       </c>
@@ -2434,33 +2434,33 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="95"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="46" t="s">
         <v>242</v>
       </c>
       <c r="E18" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
       <c r="J18" s="47" t="s">
         <v>98</v>
       </c>
       <c r="K18" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="81"/>
+      <c r="L18" s="104"/>
       <c r="M18" s="55" t="s">
         <v>163</v>
       </c>
       <c r="N18" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="O18" s="93"/>
+      <c r="O18" s="78"/>
       <c r="P18" s="52" t="s">
         <v>191</v>
       </c>
@@ -2469,31 +2469,31 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="95"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="46"/>
       <c r="E19" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="100"/>
       <c r="J19" s="47" t="s">
         <v>99</v>
       </c>
       <c r="K19" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="81"/>
+      <c r="L19" s="104"/>
       <c r="M19" s="48" t="s">
         <v>154</v>
       </c>
       <c r="N19" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="O19" s="93"/>
+      <c r="O19" s="78"/>
       <c r="P19" s="52" t="s">
         <v>192</v>
       </c>
@@ -2502,20 +2502,20 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="98"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="44">
         <v>2</v>
       </c>
-      <c r="E20" s="103" t="s">
+      <c r="E20" s="91" t="s">
         <v>150</v>
       </c>
-      <c r="F20" s="96" t="s">
+      <c r="F20" s="84" t="s">
         <v>151</v>
       </c>
-      <c r="G20" s="96"/>
+      <c r="G20" s="84"/>
       <c r="H20" s="51"/>
       <c r="J20" s="47" t="s">
         <v>105</v>
@@ -2523,14 +2523,14 @@
       <c r="K20" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="L20" s="81"/>
+      <c r="L20" s="104"/>
       <c r="M20" s="48" t="s">
         <v>155</v>
       </c>
       <c r="N20" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="O20" s="93"/>
+      <c r="O20" s="78"/>
       <c r="P20" s="47" t="s">
         <v>197</v>
       </c>
@@ -2539,12 +2539,12 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="99"/>
-      <c r="C21" s="100"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="44"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="51"/>
       <c r="J21" s="47" t="s">
         <v>100</v>
@@ -2552,14 +2552,14 @@
       <c r="K21" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="L21" s="81"/>
+      <c r="L21" s="104"/>
       <c r="M21" s="48" t="s">
         <v>156</v>
       </c>
       <c r="N21" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="O21" s="93"/>
+      <c r="O21" s="78"/>
       <c r="P21" s="52" t="s">
         <v>198</v>
       </c>
@@ -2568,12 +2568,12 @@
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="99"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="44"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="51"/>
       <c r="J22" s="32" t="s">
         <v>111</v>
@@ -2581,14 +2581,14 @@
       <c r="K22" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="L22" s="82"/>
+      <c r="L22" s="105"/>
       <c r="M22" s="48" t="s">
         <v>157</v>
       </c>
       <c r="N22" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="O22" s="93"/>
+      <c r="O22" s="78"/>
       <c r="P22" s="52" t="s">
         <v>199</v>
       </c>
@@ -2597,19 +2597,19 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="99"/>
-      <c r="C23" s="100"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="44"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
       <c r="H23" s="51"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="85"/>
-      <c r="O23" s="93"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="78"/>
       <c r="P23" s="52" t="s">
         <v>200</v>
       </c>
@@ -2618,19 +2618,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="99"/>
-      <c r="C24" s="100"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="44"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
       <c r="H24" s="51"/>
-      <c r="J24" s="86"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="93"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="78"/>
       <c r="P24" s="32" t="s">
         <v>206</v>
       </c>
@@ -2639,19 +2639,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="99"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="44"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
       <c r="H25" s="51"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="93"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="78"/>
       <c r="P25" s="32" t="s">
         <v>210</v>
       </c>
@@ -2660,19 +2660,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="99"/>
-      <c r="C26" s="100"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="44"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
       <c r="H26" s="51"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="93"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="78"/>
       <c r="P26" s="32" t="s">
         <v>211</v>
       </c>
@@ -2681,19 +2681,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="101"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="44"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
       <c r="H27" s="51"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="93"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="78"/>
       <c r="P27" s="32" t="s">
         <v>212</v>
       </c>
@@ -2702,12 +2702,12 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J28" s="86"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="88"/>
-      <c r="O28" s="93"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="78"/>
       <c r="P28" s="32" t="s">
         <v>214</v>
       </c>
@@ -2716,12 +2716,12 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J29" s="86"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="93"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="73"/>
+      <c r="O29" s="78"/>
       <c r="P29" s="32" t="s">
         <v>213</v>
       </c>
@@ -2730,12 +2730,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="86"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="88"/>
-      <c r="O30" s="93"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="78"/>
       <c r="P30" s="32" t="s">
         <v>215</v>
       </c>
@@ -2744,12 +2744,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="86"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="88"/>
-      <c r="O31" s="93"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="78"/>
       <c r="P31" s="32" t="s">
         <v>216</v>
       </c>
@@ -2758,12 +2758,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="86"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="88"/>
-      <c r="O32" s="93"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="78"/>
       <c r="P32" s="32" t="s">
         <v>217</v>
       </c>
@@ -2772,12 +2772,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="86"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="88"/>
-      <c r="O33" s="93"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="78"/>
       <c r="P33" s="32" t="s">
         <v>218</v>
       </c>
@@ -2786,12 +2786,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="86"/>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="M34" s="87"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="93"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="78"/>
       <c r="P34" s="32" t="s">
         <v>219</v>
       </c>
@@ -2800,12 +2800,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="86"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="87"/>
-      <c r="N35" s="88"/>
-      <c r="O35" s="93"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="78"/>
       <c r="P35" s="32" t="s">
         <v>220</v>
       </c>
@@ -2814,12 +2814,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="86"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-      <c r="M36" s="87"/>
-      <c r="N36" s="88"/>
-      <c r="O36" s="93"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="78"/>
       <c r="P36" s="32" t="s">
         <v>229</v>
       </c>
@@ -2828,12 +2828,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="86"/>
-      <c r="K37" s="87"/>
-      <c r="L37" s="87"/>
-      <c r="M37" s="87"/>
-      <c r="N37" s="88"/>
-      <c r="O37" s="93"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="78"/>
       <c r="P37" s="32" t="s">
         <v>230</v>
       </c>
@@ -2842,12 +2842,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="89"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="91"/>
-      <c r="O38" s="93"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="76"/>
+      <c r="O38" s="78"/>
       <c r="P38" s="32" t="s">
         <v>231</v>
       </c>
@@ -2865,18 +2865,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="J23:N38"/>
-    <mergeCell ref="O3:O38"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F20:G27"/>
-    <mergeCell ref="B20:C27"/>
-    <mergeCell ref="E20:E27"/>
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -2893,6 +2881,18 @@
     <mergeCell ref="L3:L22"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M17:N17"/>
+    <mergeCell ref="J23:N38"/>
+    <mergeCell ref="O3:O38"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F20:G27"/>
+    <mergeCell ref="B20:C27"/>
+    <mergeCell ref="E20:E27"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2924,118 +2924,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="69" t="s">
+      <c r="A1" s="100"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69" t="s">
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69" t="s">
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69" t="s">
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="81"/>
+      <c r="AE1" s="81"/>
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="81"/>
+      <c r="AK1" s="81"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="107" t="s">
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107" t="s">
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107" t="s">
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="69" t="s">
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69" t="s">
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="96" t="s">
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="S2" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="107" t="s">
+      <c r="S2" s="107" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="69" t="s">
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="94" t="s">
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="69" t="s">
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69" t="s">
+      <c r="AD2" s="81"/>
+      <c r="AE2" s="81"/>
+      <c r="AF2" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69" t="s">
+      <c r="AG2" s="81"/>
+      <c r="AH2" s="81"/>
+      <c r="AI2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="81"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3089,8 +3089,8 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="96"/>
-      <c r="S3" s="106"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="107"/>
       <c r="T3" s="16" t="s">
         <v>63</v>
       </c>
@@ -6775,12 +6775,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -6794,6 +6788,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6825,16 +6825,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6865,11 +6865,11 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="110" t="s">
+      <c r="F2" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6925,19 +6925,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -6962,16 +6962,16 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="112" t="s">
+      <c r="F6" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="113"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="112" t="s">
+      <c r="G6" s="116"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="113"/>
-      <c r="K6" s="114"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="117"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -7007,22 +7007,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="109"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -7047,21 +7047,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="110" t="s">
+      <c r="F9" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="111" t="s">
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111" t="s">
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="111"/>
-      <c r="N9" s="111"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -7115,19 +7115,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="109"/>
-      <c r="K12" s="109"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="110"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -7152,16 +7152,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="111" t="s">
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -7303,19 +7303,19 @@
       <c r="X17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="109"/>
-      <c r="J18" s="109"/>
-      <c r="K18" s="109"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
@@ -7340,16 +7340,16 @@
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="110" t="s">
+      <c r="F19" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="111" t="s">
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="111"/>
-      <c r="K19" s="111"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -7386,19 +7386,19 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="109"/>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
-      <c r="K22" s="109"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="110"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
@@ -7423,16 +7423,16 @@
       <c r="E23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="110" t="s">
+      <c r="F23" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="111" t="s">
+      <c r="G23" s="111"/>
+      <c r="H23" s="111"/>
+      <c r="I23" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
     </row>
     <row r="24" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
@@ -7468,22 +7468,22 @@
     </row>
     <row r="25" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="110"/>
     </row>
     <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
@@ -7501,44 +7501,44 @@
       <c r="E27" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="110" t="s">
+      <c r="F27" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="111" t="s">
+      <c r="G27" s="111"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111" t="s">
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109" t="s">
         <v>128</v>
       </c>
-      <c r="M27" s="111"/>
-      <c r="N27" s="111"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="109"/>
     </row>
     <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="110" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="109"/>
-      <c r="C30" s="109"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="109"/>
-      <c r="K30" s="109"/>
-      <c r="L30" s="109"/>
-      <c r="M30" s="109"/>
-      <c r="N30" s="109"/>
-      <c r="O30" s="109"/>
-      <c r="P30" s="109"/>
-      <c r="Q30" s="109"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
     </row>
     <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
@@ -7556,26 +7556,26 @@
       <c r="E31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="112" t="s">
+      <c r="F31" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="113"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="112" t="s">
+      <c r="G31" s="116"/>
+      <c r="H31" s="117"/>
+      <c r="I31" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="113"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="111" t="s">
+      <c r="J31" s="116"/>
+      <c r="K31" s="117"/>
+      <c r="L31" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="M31" s="111"/>
-      <c r="N31" s="111"/>
-      <c r="O31" s="111" t="s">
+      <c r="M31" s="109"/>
+      <c r="N31" s="109"/>
+      <c r="O31" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
+      <c r="P31" s="109"/>
+      <c r="Q31" s="109"/>
     </row>
     <row r="32" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -7598,14 +7598,14 @@
     </row>
     <row r="33" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="109"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
+      <c r="B34" s="110"/>
+      <c r="C34" s="110"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -7679,12 +7679,12 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="109" t="s">
+      <c r="A38" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -7756,15 +7756,15 @@
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="115" t="s">
+      <c r="A42" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="116"/>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="117"/>
+      <c r="B42" s="113"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+      <c r="G42" s="114"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="10"/>
@@ -7784,11 +7784,11 @@
       <c r="D43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="111" t="s">
+      <c r="E43" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="111"/>
-      <c r="G43" s="111"/>
+      <c r="F43" s="109"/>
+      <c r="G43" s="109"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="10"/>
@@ -7855,6 +7855,21 @@
     <row r="65" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="F23:H23"/>
@@ -7871,21 +7886,6 @@
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="L31:N31"/>
     <mergeCell ref="O31:Q31"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -8041,58 +8041,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
     </row>
     <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="126" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="135" t="s">
         <v>116</v>
       </c>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="128"/>
-      <c r="V2" s="133" t="s">
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="137"/>
+      <c r="V2" s="123" t="s">
         <v>124</v>
       </c>
-      <c r="W2" s="133"/>
-      <c r="X2" s="133"/>
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="133"/>
-      <c r="AA2" s="133"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
+      <c r="AA2" s="123"/>
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -8110,16 +8110,16 @@
       <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="138" t="s">
+      <c r="G3" s="125"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="139"/>
-      <c r="K3" s="140"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
       <c r="L3" s="67" t="s">
         <v>250</v>
       </c>
@@ -8138,16 +8138,16 @@
       <c r="Q3" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="R3" s="137" t="s">
+      <c r="R3" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="S3" s="137"/>
-      <c r="V3" s="133"/>
-      <c r="W3" s="133"/>
-      <c r="X3" s="133"/>
-      <c r="Y3" s="133"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="133"/>
+      <c r="S3" s="127"/>
+      <c r="V3" s="123"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+      <c r="Y3" s="123"/>
+      <c r="Z3" s="123"/>
+      <c r="AA3" s="123"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
@@ -8189,12 +8189,12 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-      <c r="V4" s="133"/>
-      <c r="W4" s="133"/>
-      <c r="X4" s="133"/>
-      <c r="Y4" s="133"/>
-      <c r="Z4" s="133"/>
-      <c r="AA4" s="133"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
@@ -8238,76 +8238,76 @@
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
       <c r="S5" s="49"/>
-      <c r="V5" s="133"/>
-      <c r="W5" s="133"/>
-      <c r="X5" s="133"/>
-      <c r="Y5" s="133"/>
-      <c r="Z5" s="133"/>
-      <c r="AA5" s="133"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="123"/>
+      <c r="Y5" s="123"/>
+      <c r="Z5" s="123"/>
+      <c r="AA5" s="123"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V6" s="133"/>
-      <c r="W6" s="133"/>
-      <c r="X6" s="133"/>
-      <c r="Y6" s="133"/>
-      <c r="Z6" s="133"/>
-      <c r="AA6" s="133"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
     </row>
     <row r="7" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="133"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
+      <c r="N7" s="133"/>
+      <c r="O7" s="133"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="123"/>
     </row>
     <row r="8" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="109"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="141" t="s">
+      <c r="A8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="O8" s="141"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="141"/>
-      <c r="R8" s="141"/>
-      <c r="V8" s="133"/>
-      <c r="W8" s="133"/>
-      <c r="X8" s="133"/>
-      <c r="Y8" s="133"/>
-      <c r="Z8" s="133"/>
-      <c r="AA8" s="133"/>
+      <c r="O8" s="131"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="131"/>
+      <c r="V8" s="123"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+      <c r="Y8" s="123"/>
+      <c r="Z8" s="123"/>
+      <c r="AA8" s="123"/>
     </row>
     <row r="9" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -8325,16 +8325,16 @@
       <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="134" t="s">
+      <c r="F9" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="135"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="138" t="s">
+      <c r="G9" s="125"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="139"/>
-      <c r="K9" s="140"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="130"/>
       <c r="L9" s="40" t="s">
         <v>115</v>
       </c>
@@ -8350,16 +8350,16 @@
       <c r="P9" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="Q9" s="134" t="s">
+      <c r="Q9" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="R9" s="136"/>
-      <c r="V9" s="133"/>
-      <c r="W9" s="133"/>
-      <c r="X9" s="133"/>
-      <c r="Y9" s="133"/>
-      <c r="Z9" s="133"/>
-      <c r="AA9" s="133"/>
+      <c r="R9" s="126"/>
+      <c r="V9" s="123"/>
+      <c r="W9" s="123"/>
+      <c r="X9" s="123"/>
+      <c r="Y9" s="123"/>
+      <c r="Z9" s="123"/>
+      <c r="AA9" s="123"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -8395,12 +8395,12 @@
         <v>40</v>
       </c>
       <c r="M10" s="26"/>
-      <c r="V10" s="133"/>
-      <c r="W10" s="133"/>
-      <c r="X10" s="133"/>
-      <c r="Y10" s="133"/>
-      <c r="Z10" s="133"/>
-      <c r="AA10" s="133"/>
+      <c r="V10" s="123"/>
+      <c r="W10" s="123"/>
+      <c r="X10" s="123"/>
+      <c r="Y10" s="123"/>
+      <c r="Z10" s="123"/>
+      <c r="AA10" s="123"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8435,51 +8435,51 @@
       <c r="L11" s="49">
         <v>40</v>
       </c>
-      <c r="V11" s="133"/>
-      <c r="W11" s="133"/>
-      <c r="X11" s="133"/>
-      <c r="Y11" s="133"/>
-      <c r="Z11" s="133"/>
-      <c r="AA11" s="133"/>
+      <c r="V11" s="123"/>
+      <c r="W11" s="123"/>
+      <c r="X11" s="123"/>
+      <c r="Y11" s="123"/>
+      <c r="Z11" s="123"/>
+      <c r="AA11" s="123"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Q12" s="49"/>
-      <c r="V12" s="133"/>
-      <c r="W12" s="133"/>
-      <c r="X12" s="133"/>
-      <c r="Y12" s="133"/>
-      <c r="Z12" s="133"/>
-      <c r="AA12" s="133"/>
+      <c r="V12" s="123"/>
+      <c r="W12" s="123"/>
+      <c r="X12" s="123"/>
+      <c r="Y12" s="123"/>
+      <c r="Z12" s="123"/>
+      <c r="AA12" s="123"/>
     </row>
     <row r="13" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="115" t="s">
+      <c r="A13" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="113"/>
       <c r="Q13" s="49"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="133"/>
-      <c r="X13" s="133"/>
-      <c r="Y13" s="133"/>
-      <c r="Z13" s="133"/>
-      <c r="AA13" s="133"/>
+      <c r="V13" s="123"/>
+      <c r="W13" s="123"/>
+      <c r="X13" s="123"/>
+      <c r="Y13" s="123"/>
+      <c r="Z13" s="123"/>
+      <c r="AA13" s="123"/>
     </row>
     <row r="14" spans="1:27" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -8497,24 +8497,24 @@
       <c r="E14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="123" t="s">
+      <c r="F14" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
       <c r="I14" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="130" t="s">
+      <c r="J14" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="131"/>
-      <c r="L14" s="132"/>
-      <c r="M14" s="129" t="s">
+      <c r="K14" s="140"/>
+      <c r="L14" s="141"/>
+      <c r="M14" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="129"/>
-      <c r="O14" s="129"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="138"/>
       <c r="P14" s="36" t="s">
         <v>80</v>
       </c>
@@ -8565,20 +8565,20 @@
       <c r="T16" s="38"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="109"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="109"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="110"/>
+      <c r="L17" s="110"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
@@ -8596,16 +8596,16 @@
       <c r="E18" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="69" t="s">
+      <c r="F18" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="94" t="s">
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="J18" s="108"/>
-      <c r="K18" s="95"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="80"/>
       <c r="L18" s="33" t="s">
         <v>162</v>
       </c>
@@ -8657,6 +8657,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="V2:AA13"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="R3:S3"/>
@@ -8668,15 +8677,6 @@
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="A7:R7"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8699,21 +8699,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="110" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="F1" s="72" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="F1" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="I1" s="72" t="s">
+      <c r="G1" s="99"/>
+      <c r="I1" s="97" t="s">
         <v>241</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="74"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
@@ -8731,12 +8731,12 @@
       <c r="G2" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="133" t="s">
+      <c r="I2" s="123" t="s">
         <v>240</v>
       </c>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="62"/>
@@ -8748,10 +8748,10 @@
       <c r="G3" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
@@ -8763,10 +8763,10 @@
       <c r="G4" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
@@ -8778,10 +8778,10 @@
       <c r="G5" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
@@ -8793,10 +8793,10 @@
       <c r="G6" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="133"/>
-      <c r="L6" s="133"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>

</xml_diff>